<commit_message>
Add unipa transcriptions (-Hasan 026)
</commit_message>
<xml_diff>
--- a/input_xlsx/Flora 001.xlsx
+++ b/input_xlsx/Flora 001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="8130" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="8130" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
@@ -2909,130 +2909,130 @@
     <t>UNIPA</t>
   </si>
   <si>
-    <t>UNIPA-2000PAD-AF001</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE001</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE002</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE003</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE004</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE005</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE006</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-VE007</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM001</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM002</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM003</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM004</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM005</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM006</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM007</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM008</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM009</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM010</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM011</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM012</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM013</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM014</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM015</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM016</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM017</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM018</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM019</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM020</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM021</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM022</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM023</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM024</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM025</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM026</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM027</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM028</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM029</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM030</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM031</t>
-  </si>
-  <si>
-    <t>UNIPA-2000PD-AF001-PM001-EM032</t>
+    <t>UNIPA-2000PD-AM001</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE001</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE002</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE003</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE004</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE005</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE006</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-VE007</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM001</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM002</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM003</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM004</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM005</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM006</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM007</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM008</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM009</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM010</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM011</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM012</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM013</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM014</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM015</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM016</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM017</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM018</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM019</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM020</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM021</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM022</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM023</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM024</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM025</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM026</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM027</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM028</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM029</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM030</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM031</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PD-AM001-PM001-EM032</t>
+  </si>
+  <si>
+    <t>UNIPA-2000PAD-AM001</t>
   </si>
 </sst>
 </file>
@@ -3743,7 +3743,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3830,10 +3830,10 @@
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" t="s">
-        <v>151</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>56</v>
@@ -3886,10 +3886,10 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
         <v>150</v>
-      </c>
-      <c r="B3" t="s">
-        <v>151</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -3957,8 +3957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD1048576"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4037,10 +4037,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
         <v>151</v>
-      </c>
-      <c r="B2" t="s">
-        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -4084,10 +4084,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -4131,10 +4131,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
         <v>94</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
         <v>94</v>
@@ -4225,10 +4225,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>94</v>
@@ -4272,10 +4272,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>94</v>
@@ -4319,10 +4319,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
         <v>94</v>
@@ -4366,10 +4366,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
         <v>94</v>
@@ -4411,10 +4411,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
         <v>94</v>
@@ -4453,10 +4453,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
         <v>94</v>
@@ -4495,10 +4495,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
         <v>94</v>
@@ -4537,10 +4537,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>94</v>
@@ -4579,10 +4579,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
         <v>94</v>
@@ -4621,10 +4621,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
         <v>94</v>
@@ -4663,10 +4663,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
         <v>94</v>
@@ -4705,10 +4705,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>94</v>
@@ -4747,10 +4747,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C18" t="s">
         <v>94</v>
@@ -4789,10 +4789,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" t="s">
         <v>94</v>
@@ -4831,10 +4831,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
         <v>94</v>
@@ -4873,10 +4873,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
         <v>94</v>
@@ -4915,10 +4915,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C22" t="s">
         <v>94</v>
@@ -4957,10 +4957,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" t="s">
         <v>94</v>
@@ -4999,10 +4999,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
@@ -5041,10 +5041,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
@@ -5083,10 +5083,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C26" t="s">
         <v>94</v>
@@ -5125,10 +5125,10 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
         <v>94</v>
@@ -5167,10 +5167,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
         <v>94</v>
@@ -5209,10 +5209,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
         <v>94</v>
@@ -5251,10 +5251,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
         <v>94</v>
@@ -5293,10 +5293,10 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C31" t="s">
         <v>94</v>
@@ -5335,10 +5335,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" t="s">
         <v>94</v>
@@ -5377,10 +5377,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
         <v>94</v>
@@ -5419,10 +5419,10 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
         <v>94</v>
@@ -5461,10 +5461,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C35" t="s">
         <v>94</v>
@@ -5503,10 +5503,10 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C36" t="s">
         <v>94</v>
@@ -5545,10 +5545,10 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C37" t="s">
         <v>94</v>
@@ -5587,10 +5587,10 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C38" t="s">
         <v>94</v>
@@ -5629,10 +5629,10 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" t="s">
         <v>94</v>
@@ -5671,10 +5671,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C40" t="s">
         <v>94</v>
@@ -5727,9 +5727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
         <v>96</v>

</xml_diff>